<commit_message>
m lay may cai file trong nay ma bo vao nek
</commit_message>
<xml_diff>
--- a/java-project-2013.xlsx
+++ b/java-project-2013.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CNTT4\Semester 1\Distributed Java\Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9915"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Giao Đồ Án 2" sheetId="2" r:id="rId2"/>
     <sheet name="DA03-HTThanh" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="242">
   <si>
     <t>ĐỒ ÁN THỰC HÀNH - 2013</t>
   </si>
@@ -732,6 +727,21 @@
   </si>
   <si>
     <t>1012370</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detail + </t>
+  </si>
+  <si>
+    <t>login</t>
   </si>
 </sst>
 </file>
@@ -943,28 +953,34 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -982,22 +998,16 @@
     <xf numFmtId="4" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1060,7 +1070,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1095,7 +1105,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1306,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1318,20 +1328,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1340,10 +1350,10 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1352,22 +1362,22 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1376,10 +1386,10 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="21"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1388,18 +1398,18 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1410,20 +1420,20 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="27"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -1449,6 +1459,9 @@
       <c r="C14" s="15">
         <v>0.5</v>
       </c>
+      <c r="D14" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
@@ -1459,6 +1472,9 @@
       </c>
       <c r="C15" s="15">
         <v>1.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1469,6 +1485,9 @@
       <c r="C16" s="15">
         <v>1</v>
       </c>
+      <c r="D16" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
@@ -1480,16 +1499,19 @@
       <c r="C17" s="15">
         <v>0.5</v>
       </c>
+      <c r="D17" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>4</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="19"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="34"/>
     </row>
     <row r="19" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
@@ -1499,6 +1521,9 @@
       <c r="C19" s="15">
         <v>0.25</v>
       </c>
+      <c r="D19" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
@@ -1508,6 +1533,9 @@
       <c r="C20" s="15">
         <v>0.25</v>
       </c>
+      <c r="D20" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
@@ -1518,6 +1546,9 @@
       </c>
       <c r="C21" s="15">
         <v>0.25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1542,11 +1573,11 @@
       <c r="A24" s="8">
         <v>6</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="19"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="34"/>
     </row>
     <row r="25" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -1578,11 +1609,11 @@
       <c r="A28" s="8">
         <v>7</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="23"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
@@ -1627,11 +1658,11 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="20"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
@@ -1706,12 +1737,12 @@
       <c r="C40" s="15"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="33"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
@@ -1831,12 +1862,12 @@
       <c r="C52" s="15"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="33"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
@@ -1889,12 +1920,12 @@
       <c r="C58" s="11"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="16"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="20"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
@@ -1966,12 +1997,12 @@
       <c r="C66" s="14"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B67" s="16"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="16"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="20"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
@@ -2173,16 +2204,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="A59:D59"/>
     <mergeCell ref="A67:D67"/>
@@ -2191,6 +2212,16 @@
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A41:D41"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2891,17 +2922,17 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="30">
+      <c r="A44" s="16">
         <v>43</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C44" s="31" t="s">
+      <c r="C44" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31" t="s">
+      <c r="D44" s="17"/>
+      <c r="E44" s="17" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>